<commit_message>
added code for ExtentReport html report, added listener and dependency
</commit_message>
<xml_diff>
--- a/target/classes/com/qa/hubspot/testdata/HubSpotTestData.xlsx
+++ b/target/classes/com/qa/hubspot/testdata/HubSpotTestData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="660" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="920" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="deals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -430,7 +431,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,4 +518,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>